<commit_message>
generated gerbers / BOMs
</commit_message>
<xml_diff>
--- a/F405_pill_V1.1/MANUFACTURE/F405_pill-top-pos.xlsx
+++ b/F405_pill_V1.1/MANUFACTURE/F405_pill-top-pos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/kicad/F405_pill/MANUFACTURE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/Documents/kicad /F405_pill/F405_pill_V1.1/MANUFACTURE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFC2EFA-DBA6-D84C-9270-AD9BD5C9E562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{150762FF-E85B-264F-836E-055A55D038F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="6480" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20780" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F405_pill-top-pos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="80">
   <si>
     <t>Val</t>
   </si>
@@ -52,7 +52,7 @@
     <t>C3</t>
   </si>
   <si>
-    <t>18p</t>
+    <t>12p</t>
   </si>
   <si>
     <t>C4</t>
@@ -199,6 +199,9 @@
     <t>R9</t>
   </si>
   <si>
+    <t>20k</t>
+  </si>
+  <si>
     <t>R10</t>
   </si>
   <si>
@@ -214,7 +217,7 @@
     <t>STM32F405RGTx</t>
   </si>
   <si>
-    <t>my_STM32F405RGTx_2</t>
+    <t>LQFP-64_10x10mm_P0.5mm</t>
   </si>
   <si>
     <t>U2</t>
@@ -1100,14 +1103,14 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1116,16 +1119,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1823,7 +1826,7 @@
         <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
         <v>51</v>
@@ -1843,10 +1846,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
         <v>51</v>
@@ -1866,10 +1869,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
         <v>61</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>51</v>
@@ -1889,13 +1892,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D35">
         <v>112.492</v>
@@ -1912,13 +1915,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D36">
         <v>137.04202799999999</v>
@@ -1935,13 +1938,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D37">
         <v>136.18199999999999</v>
@@ -1958,13 +1961,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D38">
         <v>123.33</v>

</xml_diff>